<commit_message>
Finding Text (FIND)Finding Text (FIND)
</commit_message>
<xml_diff>
--- a/Intermediate I/Week 2/workbook/W2_V4 Find.xlsx
+++ b/Intermediate I/Week 2/workbook/W2_V4 Find.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users-Data\mq20021873\Desktop\Coursera 20 April 2017\Course 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foongmin\Desktop\excel-skills-for-business\Intermediate I\Week 2\workbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D549B7A-A0B2-4E9E-A317-2ACF1CB680F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9672"/>
+    <workbookView xWindow="9580" yWindow="0" windowWidth="9620" windowHeight="5110" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,10 +18,18 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$4:$J$24</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -512,7 +521,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -933,31 +942,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4:N38"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.21875" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" customWidth="1"/>
     <col min="2" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.90625" customWidth="1"/>
+    <col min="5" max="5" width="30.08984375" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="8" max="9" width="13.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="16.109375" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" customWidth="1"/>
-    <col min="13" max="13" width="12.77734375" customWidth="1"/>
-    <col min="14" max="14" width="16.109375" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="9" width="13.6328125" customWidth="1"/>
+    <col min="10" max="10" width="17.6328125" customWidth="1"/>
+    <col min="11" max="11" width="16.08984375" customWidth="1"/>
+    <col min="12" max="12" width="10.453125" customWidth="1"/>
+    <col min="13" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="16.08984375" customWidth="1"/>
+    <col min="15" max="15" width="11.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>117</v>
       </c>
@@ -966,7 +975,7 @@
       </c>
       <c r="N1" s="8"/>
     </row>
-    <row r="3" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>90</v>
       </c>
@@ -1051,11 +1060,11 @@
         <v>2635</v>
       </c>
       <c r="N4" t="str">
-        <f>MID(K4,4,4)</f>
+        <f>MID(K4,4,FIND(" ",K4)-4)</f>
         <v>West</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1096,11 +1105,11 @@
         <v>2018</v>
       </c>
       <c r="N5" t="str">
-        <f t="shared" ref="N5:N38" si="4">MID(K5,4,4)</f>
+        <f t="shared" ref="N5:N38" si="4">MID(K5,4,FIND(" ",K5)-4)</f>
         <v>West</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -1145,7 +1154,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>108</v>
       </c>
@@ -1190,7 +1199,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>112</v>
       </c>
@@ -1235,7 +1244,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>101</v>
       </c>
@@ -1277,10 +1286,10 @@
       </c>
       <c r="N9" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -1322,10 +1331,10 @@
       </c>
       <c r="N10" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>88</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1412,10 +1421,10 @@
       </c>
       <c r="N12" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>100</v>
       </c>
@@ -1460,7 +1469,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>94</v>
       </c>
@@ -1505,7 +1514,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1547,10 +1556,10 @@
       </c>
       <c r="N15" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>93</v>
       </c>
@@ -1595,7 +1604,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1640,7 +1649,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>116</v>
       </c>
@@ -1685,7 +1694,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -1730,7 +1739,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -1775,7 +1784,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -1820,7 +1829,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -1862,10 +1871,10 @@
       </c>
       <c r="N22" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1907,10 +1916,10 @@
       </c>
       <c r="N23" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>107</v>
       </c>
@@ -1955,7 +1964,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>111</v>
       </c>
@@ -2000,7 +2009,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>89</v>
       </c>
@@ -2042,10 +2051,10 @@
       </c>
       <c r="N26" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -2087,10 +2096,10 @@
       </c>
       <c r="N27" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2135,7 +2144,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -2177,10 +2186,10 @@
       </c>
       <c r="N29" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>106</v>
       </c>
@@ -2222,10 +2231,10 @@
       </c>
       <c r="N30" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>114</v>
       </c>
@@ -2267,10 +2276,10 @@
       </c>
       <c r="N31" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>92</v>
       </c>
@@ -2312,10 +2321,10 @@
       </c>
       <c r="N32" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>113</v>
       </c>
@@ -2360,7 +2369,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -2402,10 +2411,10 @@
       </c>
       <c r="N34" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2450,7 +2459,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>109</v>
       </c>
@@ -2492,10 +2501,10 @@
       </c>
       <c r="N36" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+        <v>North</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>115</v>
       </c>
@@ -2540,7 +2549,7 @@
         <v>West</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>105</v>
       </c>
@@ -2582,11 +2591,11 @@
       </c>
       <c r="N38" t="str">
         <f t="shared" si="4"/>
-        <v>Nort</v>
+        <v>North</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:M38">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:M38">
     <sortCondition ref="B6"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>